<commit_message>
Añadir días que no habia escrito el avance, ademas de d{ia de hoy 2 de febrero
</commit_message>
<xml_diff>
--- a/Calendario practica.xlsx
+++ b/Calendario practica.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/br/Repos/practica/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bastián Romero\Documents\repos\practica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD03E82D-09D8-DB4C-8792-2EA2204C39F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDF86FD-782F-4CC0-90AC-1D39A84AD78B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{927E8441-6BF7-471D-82CE-F14F56DB68D0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{927E8441-6BF7-471D-82CE-F14F56DB68D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>Progreso de Tareas</t>
   </si>
@@ -202,9 +201,6 @@
   </si>
   <si>
     <t>Día 49</t>
-  </si>
-  <si>
-    <t>Día 50</t>
   </si>
   <si>
     <t>Objetivo: Tener sincronizadas las cámaras</t>
@@ -274,12 +270,33 @@
   <si>
     <t xml:space="preserve">Lograr visualizar la imagen de las cámaras mediante c++ para asi tener todo en ese entorno. Intentar implementar opencv para abrir cámara IP mediante un algoritmo a parte para probar la apertura de la cámara, otra posibilidad es poder abrir el video en VLC mediante sus opciones de transmisión de cámaras IP, ya que las cámaras son identificadas con una IP. Si la configuración IP en opencv no sirve, contactaré a la empresa para saber si en primer lugar es posible mostrar las imagenes mediante c++ predefinida por EVT. La ultima opción seria intentar abrir la imagen que se va guardando y mostrar solo algunos fotogramas, ahora no se si se puede renovar la imagen sin crear nuevas ventanas. </t>
   </si>
+  <si>
+    <t xml:space="preserve">Se logro visualizar la imagen en forma de video, se utilizo como base que un video es un conjunto de imágenes que se vizualisan y se refrescan a una cantidad determinada de ciclos por segundo. El problema es que al ser programación secuencial las fotografias no se toman al mismo tiempo. La idea de la sincronización es que las capturas se generan al mismo tiempo.Por eso ya se deja de lado el tema de la interfaz gráfica, aunque es importante, se debe asegurar a travez de señales externas que las cámaras actuen al mismo tiempo. </t>
+  </si>
+  <si>
+    <t>Logré ver en video dos cámaras juntas.</t>
+  </si>
+  <si>
+    <t>Reunion y preparacion de la presentacion para la reunion.</t>
+  </si>
+  <si>
+    <t>Trabajo moviendo el lab</t>
+  </si>
+  <si>
+    <t>No fui al laboratorio.</t>
+  </si>
+  <si>
+    <t>Hoy empecé a leer acerca de las entradas y salidas de la cámara, estas pueden ser utilizadas como entradas o salidas de señales para activar ciertos comportamientos. Y en general para que las lineas de tiempo de las cámaras sean iguales, esa es la idea de sincronización del sistema de cámaras.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mañana seguiré con el estudio y la lectura de los codigos de ejemplo. Una idea seria poder ingresar una señal desde una protoboard. Y poder hacer algo con la cámara mediante esa señal de entrada, por ejemplo sacar una foto cuando se hace click en un boton que deja pasar una tensión que es considerado como un nivel lógico alto. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,7 +340,7 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -354,6 +371,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -367,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -414,6 +437,8 @@
     <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,7 +457,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -730,31 +755,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3CEFCA-1939-453A-A682-61B8C78B7456}">
   <dimension ref="A2:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="140" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="32" customWidth="1"/>
-    <col min="4" max="4" width="43.5" customWidth="1"/>
-    <col min="5" max="5" width="37.1640625" customWidth="1"/>
-    <col min="6" max="6" width="26.33203125" customWidth="1"/>
+    <col min="4" max="4" width="43.42578125" customWidth="1"/>
+    <col min="5" max="5" width="37.140625" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="27" customHeight="1">
       <c r="C2" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="9"/>
     </row>
-    <row r="3" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="16.5" customHeight="1">
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="16.5" customHeight="1">
       <c r="C4" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>3</v>
@@ -763,15 +788,15 @@
         <v>5</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="71.25" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>7</v>
       </c>
@@ -785,7 +810,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="135">
       <c r="A8" s="11" t="s">
         <v>8</v>
       </c>
@@ -793,16 +818,16 @@
         <v>44210</v>
       </c>
       <c r="D8" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>59</v>
-      </c>
       <c r="F8" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="113.25" customHeight="1">
       <c r="A9" s="11" t="s">
         <v>9</v>
       </c>
@@ -810,13 +835,13 @@
         <v>44211</v>
       </c>
       <c r="D9" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="11" t="s">
         <v>10</v>
       </c>
@@ -825,7 +850,7 @@
       </c>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="11" t="s">
         <v>11</v>
       </c>
@@ -834,7 +859,7 @@
       </c>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="120">
       <c r="A12" s="11" t="s">
         <v>12</v>
       </c>
@@ -842,14 +867,14 @@
         <v>44214</v>
       </c>
       <c r="D12" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>66</v>
-      </c>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:7" ht="176" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="195">
       <c r="A13" s="11" t="s">
         <v>13</v>
       </c>
@@ -857,16 +882,16 @@
         <v>44215</v>
       </c>
       <c r="D13" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="288" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:7" ht="315">
       <c r="A14" s="11" t="s">
         <v>14</v>
       </c>
@@ -874,34 +899,34 @@
         <v>44216</v>
       </c>
       <c r="D14" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="18">
         <v>44217</v>
       </c>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="18">
         <v>44218</v>
       </c>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" s="11" t="s">
         <v>17</v>
       </c>
@@ -910,7 +935,7 @@
       </c>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" s="11" t="s">
         <v>18</v>
       </c>
@@ -919,52 +944,60 @@
       </c>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="195">
       <c r="A19" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="13">
         <v>44221</v>
       </c>
-      <c r="D19" s="8"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D19" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="19">
         <v>44222</v>
       </c>
-      <c r="D20" s="8"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D20" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="19">
         <v>44223</v>
       </c>
-      <c r="D21" s="8"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D21" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="18">
         <v>44224</v>
       </c>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="30">
       <c r="A23" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="19">
         <v>44225</v>
       </c>
-      <c r="D23" s="8"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D23" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="11" t="s">
         <v>24</v>
       </c>
@@ -973,7 +1006,7 @@
       </c>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" s="11" t="s">
         <v>25</v>
       </c>
@@ -982,282 +1015,287 @@
       </c>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="11" t="s">
-        <v>26</v>
-      </c>
+    <row r="26" spans="1:5">
+      <c r="A26" s="11"/>
       <c r="C26" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="18">
+        <v>44228</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="135">
+      <c r="A28" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="1">
-        <v>44228</v>
-      </c>
-      <c r="D27" s="8"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
+      <c r="C28" s="19">
+        <v>44229</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="1">
-        <v>44229</v>
-      </c>
-      <c r="D28" s="8"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="11" t="s">
+      <c r="C29" s="19">
+        <v>44230</v>
+      </c>
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="11" t="s">
         <v>29</v>
-      </c>
-      <c r="C29" s="1">
-        <v>44230</v>
-      </c>
-      <c r="D29" s="8"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
-        <v>30</v>
       </c>
       <c r="C30" s="1">
         <v>44231</v>
       </c>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" s="1">
         <v>44232</v>
       </c>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" s="4">
         <v>44233</v>
       </c>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33" s="4">
         <v>44234</v>
       </c>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C34" s="1">
         <v>44235</v>
       </c>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C35" s="1">
         <v>44236</v>
       </c>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C36" s="1">
         <v>44237</v>
       </c>
       <c r="D36" s="8"/>
-      <c r="E36" s="12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:5" ht="30">
       <c r="A37" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C37" s="1">
         <v>44238</v>
       </c>
       <c r="D37" s="8"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E37" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C38" s="1">
         <v>44239</v>
       </c>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C39" s="4">
         <v>44240</v>
       </c>
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C40" s="4">
         <v>44241</v>
       </c>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C41" s="1">
         <v>44242</v>
       </c>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C42" s="1">
         <v>44243</v>
       </c>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C43" s="1">
         <v>44244</v>
       </c>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C44" s="1">
         <v>44245</v>
       </c>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C45" s="1">
         <v>44246</v>
       </c>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C46" s="4">
         <v>44247</v>
       </c>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C47" s="4">
         <v>44248</v>
       </c>
       <c r="D47" s="8"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C48" s="1">
         <v>44249</v>
       </c>
       <c r="D48" s="8"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C49" s="1">
         <v>44250</v>
       </c>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C50" s="1">
         <v>44251</v>
       </c>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C51" s="1">
         <v>44252</v>
       </c>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C52" s="1">
         <v>44253</v>
       </c>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C53" s="4">
         <v>44254</v>
       </c>
       <c r="D53" s="8"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C54" s="4">
         <v>44255</v>
       </c>
       <c r="D54" s="8"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C55" s="1">
         <v>44256</v>
       </c>
       <c r="D55" s="8"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C56" s="1">
         <v>44257</v>

</xml_diff>

<commit_message>
3 de febrero trabajo en lab
</commit_message>
<xml_diff>
--- a/Calendario practica.xlsx
+++ b/Calendario practica.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bastián Romero\Documents\repos\practica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\practica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDF86FD-782F-4CC0-90AC-1D39A84AD78B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B7FA4F-A21F-4045-8AD9-DD984BC574E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{927E8441-6BF7-471D-82CE-F14F56DB68D0}"/>
   </bookViews>
@@ -755,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3CEFCA-1939-453A-A682-61B8C78B7456}">
   <dimension ref="A2:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1040,7 +1040,7 @@
       <c r="C28" s="19">
         <v>44229</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="10" t="s">
         <v>77</v>
       </c>
       <c r="E28" s="10" t="s">

</xml_diff>

<commit_message>
modificacion codigo matlab, archivos de control del lente
</commit_message>
<xml_diff>
--- a/Calendario practica.xlsx
+++ b/Calendario practica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\practica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51087763-6BF9-4312-931E-53227B25860E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F47D87-64A5-4DB2-92F8-5378DB0D7108}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{927E8441-6BF7-471D-82CE-F14F56DB68D0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
   <si>
     <t>Progreso de Tareas</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t xml:space="preserve">Optimicé el código, dentro de ciclos for uni tanto la configuracion como los parametros de la librería EVT para reducir las replicas de los codigos, así es mas sencillo configurar las camaras al menos en esta etapa donde los parametros aun no se modifican con total libertad, pero si es util para no estar comentando segmentos de codigos, cuando se puede configurar para tener cierta cantidad de camaras activadas modificando una variable. </t>
+  </si>
+  <si>
+    <t>Programar el pulsador para que inicie lás cámaras, intento de poder inciar el programa pero utilizar los parametros del software, esto no se puede ya que al utilizar hardware se utiliza el parametro del pulsador.</t>
   </si>
 </sst>
 </file>
@@ -773,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3CEFCA-1939-453A-A682-61B8C78B7456}">
   <dimension ref="A2:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F43" sqref="F41:F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1161,14 +1164,16 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" ht="30">
       <c r="A38" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C38" s="1">
         <v>44239</v>
       </c>
-      <c r="D38" s="8"/>
+      <c r="D38" s="8" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="11" t="s">
@@ -1188,14 +1193,16 @@
       </c>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" ht="75">
       <c r="A41" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C41" s="1">
         <v>44242</v>
       </c>
-      <c r="D41" s="8"/>
+      <c r="D41" s="8" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="11" t="s">
@@ -1205,6 +1212,7 @@
         <v>44243</v>
       </c>
       <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="11" t="s">
@@ -1214,6 +1222,7 @@
         <v>44244</v>
       </c>
       <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="11" t="s">
@@ -1223,6 +1232,7 @@
         <v>44245</v>
       </c>
       <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="11" t="s">
@@ -1232,6 +1242,7 @@
         <v>44246</v>
       </c>
       <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="11" t="s">

</xml_diff>